<commit_message>
Submitted to Service Science Revision 1
</commit_message>
<xml_diff>
--- a/Boeing 717-200 non-coughing.xlsx
+++ b/Boeing 717-200 non-coughing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="8">
   <si>
     <t>N</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>Optimal</t>
+  </si>
+  <si>
+    <t>Reduced</t>
+  </si>
+  <si>
+    <t>Reduced Marginal</t>
   </si>
 </sst>
 </file>
@@ -954,7 +960,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Boeing 717-200(717)'!$D$2:$D$111</c:f>
+              <c:f>'Boeing 717-200(717)'!$E$2:$E$111</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="110"/>
@@ -1031,273 +1037,273 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>180</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>360</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>540</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>720</c:v>
+                  <c:v>3.6</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>900</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1080</c:v>
+                  <c:v>5.4</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1260</c:v>
+                  <c:v>6.3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1440</c:v>
+                  <c:v>7.2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1620</c:v>
+                  <c:v>8.1</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1800</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1980</c:v>
+                  <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2160</c:v>
+                  <c:v>10.8</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2340</c:v>
+                  <c:v>11.7</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2520</c:v>
+                  <c:v>12.6</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2700</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2880</c:v>
+                  <c:v>14.4</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3060</c:v>
+                  <c:v>15.3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3240</c:v>
+                  <c:v>16.2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3420</c:v>
+                  <c:v>17.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3600</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3780</c:v>
+                  <c:v>18.899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3960</c:v>
+                  <c:v>19.8</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4140</c:v>
+                  <c:v>20.7</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4320</c:v>
+                  <c:v>21.6</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4680</c:v>
+                  <c:v>23.4</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>5040</c:v>
+                  <c:v>25.2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>5580</c:v>
+                  <c:v>27.9</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>6120</c:v>
+                  <c:v>30.6</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>6660</c:v>
+                  <c:v>33.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>7200</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>7740</c:v>
+                  <c:v>38.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>8280</c:v>
+                  <c:v>41.4</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>8820</c:v>
+                  <c:v>44.1</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>9360</c:v>
+                  <c:v>46.8</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>9900</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>10440</c:v>
+                  <c:v>52.2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>10980</c:v>
+                  <c:v>54.9</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>11700</c:v>
+                  <c:v>58.5</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>12420</c:v>
+                  <c:v>62.1</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>13140</c:v>
+                  <c:v>65.7</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>13860</c:v>
+                  <c:v>69.3</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>14580</c:v>
+                  <c:v>72.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>15300</c:v>
+                  <c:v>76.5</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>16020</c:v>
+                  <c:v>80.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>16740</c:v>
+                  <c:v>83.7</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>17460</c:v>
+                  <c:v>87.3</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>18180</c:v>
+                  <c:v>90.9</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>19080</c:v>
+                  <c:v>95.4</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>19980</c:v>
+                  <c:v>99.9</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>20880</c:v>
+                  <c:v>104.4</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>21780</c:v>
+                  <c:v>108.9</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>22680</c:v>
+                  <c:v>113.4</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>23760</c:v>
+                  <c:v>118.8</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>24660</c:v>
+                  <c:v>123.3</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>25740</c:v>
+                  <c:v>128.69999999999999</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>26640</c:v>
+                  <c:v>133.19999999999999</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>27720</c:v>
+                  <c:v>138.6</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>28620</c:v>
+                  <c:v>143.1</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>29700</c:v>
+                  <c:v>148.5</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>30600</c:v>
+                  <c:v>153</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>31680</c:v>
+                  <c:v>158.4</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>32580</c:v>
+                  <c:v>162.9</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>33660</c:v>
+                  <c:v>168.3</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>34560</c:v>
+                  <c:v>172.8</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>35640</c:v>
+                  <c:v>178.2</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>36720</c:v>
+                  <c:v>183.6</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>37800</c:v>
+                  <c:v>189</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>38880</c:v>
+                  <c:v>194.4</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>40320</c:v>
+                  <c:v>201.6</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>41760</c:v>
+                  <c:v>208.8</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>43380</c:v>
+                  <c:v>216.9</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>45000</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>46620</c:v>
+                  <c:v>233.1</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>48240</c:v>
+                  <c:v>241.2</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>49860</c:v>
+                  <c:v>249.3</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>51480</c:v>
+                  <c:v>257.39999999999998</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>53280</c:v>
+                  <c:v>266.39999999999998</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>55080</c:v>
+                  <c:v>275.39999999999998</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>57060</c:v>
+                  <c:v>285.3</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>59040</c:v>
+                  <c:v>295.2</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>61020</c:v>
+                  <c:v>305.10000000000002</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>63000</c:v>
+                  <c:v>315</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>64980</c:v>
+                  <c:v>324.89999999999998</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>66960</c:v>
+                  <c:v>334.8</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>68940</c:v>
+                  <c:v>344.7</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>70920</c:v>
+                  <c:v>354.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="132228992"/>
-        <c:axId val="132235648"/>
+        <c:axId val="120448896"/>
+        <c:axId val="120656256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="132228992"/>
+        <c:axId val="120448896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1336,14 +1342,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132235648"/>
+        <c:crossAx val="120656256"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132235648"/>
+        <c:axId val="120656256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1383,7 +1389,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132228992"/>
+        <c:crossAx val="120448896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1392,7 +1398,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1429,7 +1435,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Boeing 717-200(717)'!$E$1</c:f>
+              <c:f>'Boeing 717-200(717)'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1779,7 +1785,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Boeing 717-200(717)'!$E$2:$E$111</c:f>
+              <c:f>'Boeing 717-200(717)'!$G$2:$G$111</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="110"/>
@@ -1853,273 +1859,273 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>180</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>180</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>180</c:v>
+                  <c:v>0.90000000000000013</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>180</c:v>
+                  <c:v>0.89999999999999991</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>180</c:v>
+                  <c:v>0.89999999999999991</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>180</c:v>
+                  <c:v>0.90000000000000036</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>180</c:v>
+                  <c:v>0.89999999999999947</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>180</c:v>
+                  <c:v>0.90000000000000036</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>180</c:v>
+                  <c:v>0.89999999999999947</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>180</c:v>
+                  <c:v>0.90000000000000036</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>180</c:v>
+                  <c:v>0.90000000000000036</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>180</c:v>
+                  <c:v>0.90000000000000036</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>180</c:v>
+                  <c:v>0.89999999999999858</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>180</c:v>
+                  <c:v>0.90000000000000036</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>180</c:v>
+                  <c:v>0.90000000000000036</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>180</c:v>
+                  <c:v>0.90000000000000036</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>180</c:v>
+                  <c:v>0.90000000000000036</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>180</c:v>
+                  <c:v>0.89999999999999858</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>180</c:v>
+                  <c:v>0.90000000000000213</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>180</c:v>
+                  <c:v>0.89999999999999858</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>180</c:v>
+                  <c:v>0.89999999999999858</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>180</c:v>
+                  <c:v>0.90000000000000213</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>180</c:v>
+                  <c:v>0.89999999999999858</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>180</c:v>
+                  <c:v>0.90000000000000213</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>360</c:v>
+                  <c:v>1.7999999999999972</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>360</c:v>
+                  <c:v>1.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>540</c:v>
+                  <c:v>2.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>540</c:v>
+                  <c:v>2.7000000000000028</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>540</c:v>
+                  <c:v>2.6999999999999957</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>540</c:v>
+                  <c:v>2.7000000000000028</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>540</c:v>
+                  <c:v>2.7000000000000028</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>540</c:v>
+                  <c:v>2.6999999999999957</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>540</c:v>
+                  <c:v>2.7000000000000028</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>540</c:v>
+                  <c:v>2.6999999999999957</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>540</c:v>
+                  <c:v>2.7000000000000028</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>540</c:v>
+                  <c:v>2.7000000000000028</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>540</c:v>
+                  <c:v>2.6999999999999957</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>720</c:v>
+                  <c:v>3.6000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>720</c:v>
+                  <c:v>3.6000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>720</c:v>
+                  <c:v>3.6000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>720</c:v>
+                  <c:v>3.5999999999999943</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>720</c:v>
+                  <c:v>3.6000000000000085</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>720</c:v>
+                  <c:v>3.5999999999999943</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>720</c:v>
+                  <c:v>3.5999999999999943</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>720</c:v>
+                  <c:v>3.6000000000000085</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>720</c:v>
+                  <c:v>3.5999999999999943</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>720</c:v>
+                  <c:v>3.6000000000000085</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>900</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>900</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>900</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>900</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>900</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1080</c:v>
+                  <c:v>5.3999999999999915</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>900</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1080</c:v>
+                  <c:v>5.3999999999999915</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>900</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1080</c:v>
+                  <c:v>5.4000000000000057</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>900</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1080</c:v>
+                  <c:v>5.4000000000000057</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>900</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1080</c:v>
+                  <c:v>5.4000000000000057</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>900</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1080</c:v>
+                  <c:v>5.4000000000000057</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>900</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1080</c:v>
+                  <c:v>5.3999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1080</c:v>
+                  <c:v>5.4000000000000057</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1080</c:v>
+                  <c:v>5.4000000000000057</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1080</c:v>
+                  <c:v>5.4000000000000057</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1440</c:v>
+                  <c:v>7.1999999999999886</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1440</c:v>
+                  <c:v>7.2000000000000171</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1620</c:v>
+                  <c:v>8.0999999999999943</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1620</c:v>
+                  <c:v>8.0999999999999943</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1620</c:v>
+                  <c:v>8.0999999999999943</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1620</c:v>
+                  <c:v>8.0999999999999943</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1620</c:v>
+                  <c:v>8.1000000000000227</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1620</c:v>
+                  <c:v>8.0999999999999659</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1800</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>1800</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>1980</c:v>
+                  <c:v>9.9000000000000341</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>1980</c:v>
+                  <c:v>9.8999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>1980</c:v>
+                  <c:v>9.9000000000000341</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>1980</c:v>
+                  <c:v>9.8999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>1980</c:v>
+                  <c:v>9.8999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>1980</c:v>
+                  <c:v>9.9000000000000341</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1980</c:v>
+                  <c:v>9.8999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>1980</c:v>
+                  <c:v>9.9000000000000341</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="132591616"/>
-        <c:axId val="132593536"/>
+        <c:axId val="120676352"/>
+        <c:axId val="120678272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="132591616"/>
+        <c:axId val="120676352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2158,17 +2164,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132593536"/>
+        <c:crossAx val="120678272"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132593536"/>
+        <c:axId val="120678272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2000"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
@@ -2211,7 +2216,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132591616"/>
+        <c:crossAx val="120676352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2220,7 +2225,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2946,11 +2951,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="132617728"/>
-        <c:axId val="132619648"/>
+        <c:axId val="120714752"/>
+        <c:axId val="120716672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="132617728"/>
+        <c:axId val="120714752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2989,14 +2994,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132619648"/>
+        <c:crossAx val="120716672"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132619648"/>
+        <c:axId val="120716672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3041,7 +3046,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132617728"/>
+        <c:crossAx val="120714752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3050,7 +3055,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3060,13 +3065,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
@@ -3090,13 +3095,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>586740</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>541020</xdr:colOff>
       <xdr:row>93</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -3120,13 +3125,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>579120</xdr:colOff>
       <xdr:row>95</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>142</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3436,15 +3441,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E111"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3458,10 +3463,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3474,8 +3485,12 @@
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2">
+        <f>D2/200</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3489,11 +3504,19 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E34" si="0">D3 - D2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <f t="shared" ref="E3:E66" si="0">D3/200</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:G34" si="1">D3 - D2</f>
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3510,8 +3533,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3528,8 +3559,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3546,8 +3585,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3564,8 +3611,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3582,8 +3637,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3600,8 +3663,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3618,8 +3689,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3636,8 +3715,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3654,8 +3741,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3672,8 +3767,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3690,8 +3793,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3708,8 +3819,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3726,8 +3845,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3744,8 +3871,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3762,8 +3897,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3780,8 +3923,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3798,8 +3949,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3816,8 +3975,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3834,8 +4001,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3852,8 +4027,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3870,8 +4053,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3888,8 +4079,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3904,10 +4103,18 @@
       </c>
       <c r="E26">
         <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3922,10 +4129,18 @@
       </c>
       <c r="E27">
         <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3940,10 +4155,18 @@
       </c>
       <c r="E28">
         <f t="shared" si="0"/>
+        <v>2.7</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>0.90000000000000013</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3958,10 +4181,18 @@
       </c>
       <c r="E29">
         <f t="shared" si="0"/>
+        <v>3.6</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>0.89999999999999991</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3976,10 +4207,18 @@
       </c>
       <c r="E30">
         <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>0.89999999999999991</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3994,10 +4233,18 @@
       </c>
       <c r="E31">
         <f t="shared" si="0"/>
+        <v>5.4</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>0.90000000000000036</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4012,10 +4259,18 @@
       </c>
       <c r="E32">
         <f t="shared" si="0"/>
+        <v>6.3</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>0.89999999999999947</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4030,10 +4285,18 @@
       </c>
       <c r="E33">
         <f t="shared" si="0"/>
+        <v>7.2</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>0.90000000000000036</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4048,10 +4311,18 @@
       </c>
       <c r="E34">
         <f t="shared" si="0"/>
+        <v>8.1</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>0.89999999999999947</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4065,11 +4336,19 @@
         <v>1800</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E35:E66" si="1">D35 - D34</f>
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F35">
+        <f t="shared" ref="F35:G66" si="2">D35 - D34</f>
         <v>180</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="G35">
+        <f t="shared" si="2"/>
+        <v>0.90000000000000036</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4083,11 +4362,19 @@
         <v>1980</v>
       </c>
       <c r="E36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>9.9</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="G36">
+        <f t="shared" si="2"/>
+        <v>0.90000000000000036</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4101,11 +4388,19 @@
         <v>2160</v>
       </c>
       <c r="E37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>10.8</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="G37">
+        <f t="shared" si="2"/>
+        <v>0.90000000000000036</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4119,11 +4414,19 @@
         <v>2340</v>
       </c>
       <c r="E38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>11.7</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="G38">
+        <f t="shared" si="2"/>
+        <v>0.89999999999999858</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4137,11 +4440,19 @@
         <v>2520</v>
       </c>
       <c r="E39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>12.6</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="G39">
+        <f t="shared" si="2"/>
+        <v>0.90000000000000036</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4155,11 +4466,19 @@
         <v>2700</v>
       </c>
       <c r="E40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>13.5</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="G40">
+        <f t="shared" si="2"/>
+        <v>0.90000000000000036</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4173,11 +4492,19 @@
         <v>2880</v>
       </c>
       <c r="E41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>14.4</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="G41">
+        <f t="shared" si="2"/>
+        <v>0.90000000000000036</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4191,11 +4518,19 @@
         <v>3060</v>
       </c>
       <c r="E42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>15.3</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="G42">
+        <f t="shared" si="2"/>
+        <v>0.90000000000000036</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4209,11 +4544,19 @@
         <v>3240</v>
       </c>
       <c r="E43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>16.2</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="G43">
+        <f t="shared" si="2"/>
+        <v>0.89999999999999858</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4227,11 +4570,19 @@
         <v>3420</v>
       </c>
       <c r="E44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>17.100000000000001</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="G44">
+        <f t="shared" si="2"/>
+        <v>0.90000000000000213</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4245,11 +4596,19 @@
         <v>3600</v>
       </c>
       <c r="E45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="G45">
+        <f t="shared" si="2"/>
+        <v>0.89999999999999858</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4263,11 +4622,19 @@
         <v>3780</v>
       </c>
       <c r="E46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>18.899999999999999</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="G46">
+        <f t="shared" si="2"/>
+        <v>0.89999999999999858</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4281,11 +4648,19 @@
         <v>3960</v>
       </c>
       <c r="E47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>19.8</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="G47">
+        <f t="shared" si="2"/>
+        <v>0.90000000000000213</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4299,11 +4674,19 @@
         <v>4140</v>
       </c>
       <c r="E48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>20.7</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="G48">
+        <f t="shared" si="2"/>
+        <v>0.89999999999999858</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4317,11 +4700,19 @@
         <v>4320</v>
       </c>
       <c r="E49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>21.6</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="G49">
+        <f t="shared" si="2"/>
+        <v>0.90000000000000213</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4335,11 +4726,19 @@
         <v>4680</v>
       </c>
       <c r="E50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>23.4</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="2"/>
         <v>360</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="G50">
+        <f t="shared" si="2"/>
+        <v>1.7999999999999972</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4353,11 +4752,19 @@
         <v>5040</v>
       </c>
       <c r="E51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>25.2</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="2"/>
         <v>360</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="G51">
+        <f t="shared" si="2"/>
+        <v>1.8000000000000007</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4371,11 +4778,19 @@
         <v>5580</v>
       </c>
       <c r="E52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>27.9</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="2"/>
         <v>540</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="G52">
+        <f t="shared" si="2"/>
+        <v>2.6999999999999993</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4389,11 +4804,19 @@
         <v>6120</v>
       </c>
       <c r="E53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>30.6</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="2"/>
         <v>540</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="G53">
+        <f t="shared" si="2"/>
+        <v>2.7000000000000028</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4407,11 +4830,19 @@
         <v>6660</v>
       </c>
       <c r="E54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>33.299999999999997</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="2"/>
         <v>540</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="G54">
+        <f t="shared" si="2"/>
+        <v>2.6999999999999957</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4425,11 +4856,19 @@
         <v>7200</v>
       </c>
       <c r="E55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="2"/>
         <v>540</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="G55">
+        <f t="shared" si="2"/>
+        <v>2.7000000000000028</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4443,11 +4882,19 @@
         <v>7740</v>
       </c>
       <c r="E56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>38.700000000000003</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="2"/>
         <v>540</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="G56">
+        <f t="shared" si="2"/>
+        <v>2.7000000000000028</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4461,11 +4908,19 @@
         <v>8280</v>
       </c>
       <c r="E57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>41.4</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="2"/>
         <v>540</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="G57">
+        <f t="shared" si="2"/>
+        <v>2.6999999999999957</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4479,11 +4934,19 @@
         <v>8820</v>
       </c>
       <c r="E58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>44.1</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="2"/>
         <v>540</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="G58">
+        <f t="shared" si="2"/>
+        <v>2.7000000000000028</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4497,11 +4960,19 @@
         <v>9360</v>
       </c>
       <c r="E59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>46.8</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="2"/>
         <v>540</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="G59">
+        <f t="shared" si="2"/>
+        <v>2.6999999999999957</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4515,11 +4986,19 @@
         <v>9900</v>
       </c>
       <c r="E60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>49.5</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="2"/>
         <v>540</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="G60">
+        <f t="shared" si="2"/>
+        <v>2.7000000000000028</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4533,11 +5012,19 @@
         <v>10440</v>
       </c>
       <c r="E61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>52.2</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="2"/>
         <v>540</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="G61">
+        <f t="shared" si="2"/>
+        <v>2.7000000000000028</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4551,11 +5038,19 @@
         <v>10980</v>
       </c>
       <c r="E62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>54.9</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="2"/>
         <v>540</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="G62">
+        <f t="shared" si="2"/>
+        <v>2.6999999999999957</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4569,11 +5064,19 @@
         <v>11700</v>
       </c>
       <c r="E63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>58.5</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="2"/>
         <v>720</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="G63">
+        <f t="shared" si="2"/>
+        <v>3.6000000000000014</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4587,11 +5090,19 @@
         <v>12420</v>
       </c>
       <c r="E64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>62.1</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="2"/>
         <v>720</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="G64">
+        <f t="shared" si="2"/>
+        <v>3.6000000000000014</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4605,11 +5116,19 @@
         <v>13140</v>
       </c>
       <c r="E65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>65.7</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="2"/>
         <v>720</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="G65">
+        <f t="shared" si="2"/>
+        <v>3.6000000000000014</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4623,11 +5142,19 @@
         <v>13860</v>
       </c>
       <c r="E66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="2"/>
         <v>720</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="G66">
+        <f t="shared" si="2"/>
+        <v>3.5999999999999943</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4641,11 +5168,19 @@
         <v>14580</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E98" si="2">D67 - D66</f>
+        <f t="shared" ref="E67:E111" si="3">D67/200</f>
+        <v>72.900000000000006</v>
+      </c>
+      <c r="F67">
+        <f t="shared" ref="F67:G98" si="4">D67 - D66</f>
         <v>720</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="G67">
+        <f t="shared" si="4"/>
+        <v>3.6000000000000085</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4659,11 +5194,19 @@
         <v>15300</v>
       </c>
       <c r="E68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>76.5</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="4"/>
         <v>720</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="G68">
+        <f t="shared" si="4"/>
+        <v>3.5999999999999943</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4677,11 +5220,19 @@
         <v>16020</v>
       </c>
       <c r="E69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>80.099999999999994</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="4"/>
         <v>720</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="G69">
+        <f t="shared" si="4"/>
+        <v>3.5999999999999943</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4695,11 +5246,19 @@
         <v>16740</v>
       </c>
       <c r="E70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>83.7</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="4"/>
         <v>720</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="G70">
+        <f t="shared" si="4"/>
+        <v>3.6000000000000085</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4713,11 +5272,19 @@
         <v>17460</v>
       </c>
       <c r="E71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>87.3</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="4"/>
         <v>720</v>
       </c>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="G71">
+        <f t="shared" si="4"/>
+        <v>3.5999999999999943</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4731,11 +5298,19 @@
         <v>18180</v>
       </c>
       <c r="E72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>90.9</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="4"/>
         <v>720</v>
       </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="G72">
+        <f t="shared" si="4"/>
+        <v>3.6000000000000085</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4749,11 +5324,19 @@
         <v>19080</v>
       </c>
       <c r="E73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>95.4</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="G73">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4767,11 +5350,19 @@
         <v>19980</v>
       </c>
       <c r="E74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>99.9</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="G74">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4785,11 +5376,19 @@
         <v>20880</v>
       </c>
       <c r="E75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>104.4</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="G75">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4803,11 +5402,19 @@
         <v>21780</v>
       </c>
       <c r="E76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>108.9</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="G76">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4821,11 +5428,19 @@
         <v>22680</v>
       </c>
       <c r="E77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>113.4</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
-    </row>
-    <row r="78" spans="1:5">
+      <c r="G77">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4839,11 +5454,19 @@
         <v>23760</v>
       </c>
       <c r="E78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>118.8</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="4"/>
         <v>1080</v>
       </c>
-    </row>
-    <row r="79" spans="1:5">
+      <c r="G78">
+        <f t="shared" si="4"/>
+        <v>5.3999999999999915</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4857,11 +5480,19 @@
         <v>24660</v>
       </c>
       <c r="E79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>123.3</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
-    </row>
-    <row r="80" spans="1:5">
+      <c r="G79">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4875,11 +5506,19 @@
         <v>25740</v>
       </c>
       <c r="E80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>128.69999999999999</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="4"/>
         <v>1080</v>
       </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="G80">
+        <f t="shared" si="4"/>
+        <v>5.3999999999999915</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4893,11 +5532,19 @@
         <v>26640</v>
       </c>
       <c r="E81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>133.19999999999999</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="G81">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4911,11 +5558,19 @@
         <v>27720</v>
       </c>
       <c r="E82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>138.6</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="4"/>
         <v>1080</v>
       </c>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="G82">
+        <f t="shared" si="4"/>
+        <v>5.4000000000000057</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4929,11 +5584,19 @@
         <v>28620</v>
       </c>
       <c r="E83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>143.1</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="G83">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4947,11 +5610,19 @@
         <v>29700</v>
       </c>
       <c r="E84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>148.5</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="4"/>
         <v>1080</v>
       </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="G84">
+        <f t="shared" si="4"/>
+        <v>5.4000000000000057</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4965,11 +5636,19 @@
         <v>30600</v>
       </c>
       <c r="E85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>153</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="G85">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4983,11 +5662,19 @@
         <v>31680</v>
       </c>
       <c r="E86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>158.4</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="4"/>
         <v>1080</v>
       </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="G86">
+        <f t="shared" si="4"/>
+        <v>5.4000000000000057</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5001,11 +5688,19 @@
         <v>32580</v>
       </c>
       <c r="E87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>162.9</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="G87">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5019,11 +5714,19 @@
         <v>33660</v>
       </c>
       <c r="E88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>168.3</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="4"/>
         <v>1080</v>
       </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="G88">
+        <f t="shared" si="4"/>
+        <v>5.4000000000000057</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5037,11 +5740,19 @@
         <v>34560</v>
       </c>
       <c r="E89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>172.8</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
-    </row>
-    <row r="90" spans="1:5">
+      <c r="G89">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5055,11 +5766,19 @@
         <v>35640</v>
       </c>
       <c r="E90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>178.2</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="4"/>
         <v>1080</v>
       </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="G90">
+        <f t="shared" si="4"/>
+        <v>5.3999999999999773</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5073,11 +5792,19 @@
         <v>36720</v>
       </c>
       <c r="E91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>183.6</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="4"/>
         <v>1080</v>
       </c>
-    </row>
-    <row r="92" spans="1:5">
+      <c r="G91">
+        <f t="shared" si="4"/>
+        <v>5.4000000000000057</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5091,11 +5818,19 @@
         <v>37800</v>
       </c>
       <c r="E92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>189</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="4"/>
         <v>1080</v>
       </c>
-    </row>
-    <row r="93" spans="1:5">
+      <c r="G92">
+        <f t="shared" si="4"/>
+        <v>5.4000000000000057</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5109,11 +5844,19 @@
         <v>38880</v>
       </c>
       <c r="E93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>194.4</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="4"/>
         <v>1080</v>
       </c>
-    </row>
-    <row r="94" spans="1:5">
+      <c r="G93">
+        <f t="shared" si="4"/>
+        <v>5.4000000000000057</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5127,11 +5870,19 @@
         <v>40320</v>
       </c>
       <c r="E94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>201.6</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="4"/>
         <v>1440</v>
       </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="G94">
+        <f t="shared" si="4"/>
+        <v>7.1999999999999886</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5145,11 +5896,19 @@
         <v>41760</v>
       </c>
       <c r="E95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>208.8</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="4"/>
         <v>1440</v>
       </c>
-    </row>
-    <row r="96" spans="1:5">
+      <c r="G95">
+        <f t="shared" si="4"/>
+        <v>7.2000000000000171</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5163,11 +5922,19 @@
         <v>43380</v>
       </c>
       <c r="E96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>216.9</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="4"/>
         <v>1620</v>
       </c>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="G96">
+        <f t="shared" si="4"/>
+        <v>8.0999999999999943</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5181,11 +5948,19 @@
         <v>45000</v>
       </c>
       <c r="E97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>225</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="4"/>
         <v>1620</v>
       </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="G97">
+        <f t="shared" si="4"/>
+        <v>8.0999999999999943</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5199,11 +5974,19 @@
         <v>46620</v>
       </c>
       <c r="E98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>233.1</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="4"/>
         <v>1620</v>
       </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="G98">
+        <f t="shared" si="4"/>
+        <v>8.0999999999999943</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99">
         <v>98</v>
       </c>
@@ -5217,11 +6000,19 @@
         <v>48240</v>
       </c>
       <c r="E99">
-        <f t="shared" ref="E99:E111" si="3">D99 - D98</f>
+        <f t="shared" si="3"/>
+        <v>241.2</v>
+      </c>
+      <c r="F99">
+        <f t="shared" ref="F99:G111" si="5">D99 - D98</f>
         <v>1620</v>
       </c>
-    </row>
-    <row r="100" spans="1:5">
+      <c r="G99">
+        <f t="shared" si="5"/>
+        <v>8.0999999999999943</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5236,10 +6027,18 @@
       </c>
       <c r="E100">
         <f t="shared" si="3"/>
+        <v>249.3</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="5"/>
         <v>1620</v>
       </c>
-    </row>
-    <row r="101" spans="1:5">
+      <c r="G100">
+        <f t="shared" si="5"/>
+        <v>8.1000000000000227</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101">
         <v>100</v>
       </c>
@@ -5254,10 +6053,18 @@
       </c>
       <c r="E101">
         <f t="shared" si="3"/>
+        <v>257.39999999999998</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="5"/>
         <v>1620</v>
       </c>
-    </row>
-    <row r="102" spans="1:5">
+      <c r="G101">
+        <f t="shared" si="5"/>
+        <v>8.0999999999999659</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
       <c r="A102">
         <v>101</v>
       </c>
@@ -5272,10 +6079,18 @@
       </c>
       <c r="E102">
         <f t="shared" si="3"/>
+        <v>266.39999999999998</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="5"/>
         <v>1800</v>
       </c>
-    </row>
-    <row r="103" spans="1:5">
+      <c r="G102">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
       <c r="A103">
         <v>102</v>
       </c>
@@ -5290,10 +6105,18 @@
       </c>
       <c r="E103">
         <f t="shared" si="3"/>
+        <v>275.39999999999998</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="5"/>
         <v>1800</v>
       </c>
-    </row>
-    <row r="104" spans="1:5">
+      <c r="G103">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104">
         <v>103</v>
       </c>
@@ -5308,10 +6131,18 @@
       </c>
       <c r="E104">
         <f t="shared" si="3"/>
+        <v>285.3</v>
+      </c>
+      <c r="F104">
+        <f t="shared" si="5"/>
         <v>1980</v>
       </c>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="G104">
+        <f t="shared" si="5"/>
+        <v>9.9000000000000341</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
       <c r="A105">
         <v>104</v>
       </c>
@@ -5326,10 +6157,18 @@
       </c>
       <c r="E105">
         <f t="shared" si="3"/>
+        <v>295.2</v>
+      </c>
+      <c r="F105">
+        <f t="shared" si="5"/>
         <v>1980</v>
       </c>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="G105">
+        <f t="shared" si="5"/>
+        <v>9.8999999999999773</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
       <c r="A106">
         <v>105</v>
       </c>
@@ -5344,10 +6183,18 @@
       </c>
       <c r="E106">
         <f t="shared" si="3"/>
+        <v>305.10000000000002</v>
+      </c>
+      <c r="F106">
+        <f t="shared" si="5"/>
         <v>1980</v>
       </c>
-    </row>
-    <row r="107" spans="1:5">
+      <c r="G106">
+        <f t="shared" si="5"/>
+        <v>9.9000000000000341</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
       <c r="A107">
         <v>106</v>
       </c>
@@ -5362,10 +6209,18 @@
       </c>
       <c r="E107">
         <f t="shared" si="3"/>
+        <v>315</v>
+      </c>
+      <c r="F107">
+        <f t="shared" si="5"/>
         <v>1980</v>
       </c>
-    </row>
-    <row r="108" spans="1:5">
+      <c r="G107">
+        <f t="shared" si="5"/>
+        <v>9.8999999999999773</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
       <c r="A108">
         <v>107</v>
       </c>
@@ -5380,10 +6235,18 @@
       </c>
       <c r="E108">
         <f t="shared" si="3"/>
+        <v>324.89999999999998</v>
+      </c>
+      <c r="F108">
+        <f t="shared" si="5"/>
         <v>1980</v>
       </c>
-    </row>
-    <row r="109" spans="1:5">
+      <c r="G108">
+        <f t="shared" si="5"/>
+        <v>9.8999999999999773</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
       <c r="A109">
         <v>108</v>
       </c>
@@ -5398,10 +6261,18 @@
       </c>
       <c r="E109">
         <f t="shared" si="3"/>
+        <v>334.8</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="5"/>
         <v>1980</v>
       </c>
-    </row>
-    <row r="110" spans="1:5">
+      <c r="G109">
+        <f t="shared" si="5"/>
+        <v>9.9000000000000341</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
       <c r="A110">
         <v>109</v>
       </c>
@@ -5416,10 +6287,18 @@
       </c>
       <c r="E110">
         <f t="shared" si="3"/>
+        <v>344.7</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="5"/>
         <v>1980</v>
       </c>
-    </row>
-    <row r="111" spans="1:5">
+      <c r="G110">
+        <f t="shared" si="5"/>
+        <v>9.8999999999999773</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
       <c r="A111">
         <v>110</v>
       </c>
@@ -5434,7 +6313,15 @@
       </c>
       <c r="E111">
         <f t="shared" si="3"/>
+        <v>354.6</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="5"/>
         <v>1980</v>
+      </c>
+      <c r="G111">
+        <f t="shared" si="5"/>
+        <v>9.9000000000000341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>